<commit_message>
Sudah Pengolahan Data dan Ada File Rangkuman Jurnal
</commit_message>
<xml_diff>
--- a/Perhitungan K-Means K_3.xlsx
+++ b/Perhitungan K-Means K_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CADANGAN SKRIPSI GIT HUB\DATA SKRIPSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82048860-7419-40FB-A5C4-26ABE305EF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0C651B-21A4-4B84-86D6-B807F99C7A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{204938CF-0984-440D-97FB-7D0080130912}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Lembar2" sheetId="2" r:id="rId2"/>
     <sheet name="CURANMOR" sheetId="3" r:id="rId3"/>
     <sheet name="CURAS" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="60">
   <si>
     <t>DATA CURAS DAN CURANMOR KAB PROBOLINGGO 2021 - 2022</t>
   </si>
@@ -379,6 +380,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -387,9 +391,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -724,53 +725,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C2" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="C2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J3" s="34" t="s">
+      <c r="J3" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="33">
+      <c r="B5" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="34">
         <v>2021</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33">
+      <c r="D5" s="34"/>
+      <c r="E5" s="34">
         <v>2022</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="34"/>
+      <c r="G5" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" s="33">
+      <c r="J5" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="34">
         <v>2021</v>
       </c>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33">
+      <c r="L5" s="34"/>
+      <c r="M5" s="34">
         <v>2022</v>
       </c>
-      <c r="N5" s="33"/>
+      <c r="N5" s="34"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="33"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
@@ -783,8 +784,8 @@
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="J6" s="33"/>
+      <c r="G6" s="34"/>
+      <c r="J6" s="34"/>
       <c r="K6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1814,23 +1815,23 @@
       <c r="B32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="33">
+      <c r="C32" s="34">
         <f>C31+D31</f>
         <v>219</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33">
+      <c r="D32" s="34"/>
+      <c r="E32" s="34">
         <f>E31+F31</f>
         <v>178</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="J32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K32" s="33"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="33"/>
-      <c r="N32" s="33"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="34"/>
     </row>
     <row r="33" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
@@ -1932,19 +1933,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="C2" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
       <c r="L3" t="s">
         <v>31</v>
       </c>
@@ -1953,12 +1954,12 @@
       </c>
     </row>
     <row r="4" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="L4" s="34" t="s">
+      <c r="L4" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
       <c r="R4" s="27" t="s">
         <v>46</v>
       </c>
@@ -2002,14 +2003,14 @@
       <c r="BG4" s="27"/>
     </row>
     <row r="5" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="33">
+      <c r="B5" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="34">
         <v>2024</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33" t="s">
+      <c r="D5" s="34"/>
+      <c r="E5" s="34" t="s">
         <v>28</v>
       </c>
       <c r="H5" s="4"/>
@@ -2092,14 +2093,14 @@
       <c r="BG5" s="27"/>
     </row>
     <row r="6" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="B6" s="33"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="33"/>
+      <c r="E6" s="34"/>
       <c r="H6" s="4" t="s">
         <v>1</v>
       </c>
@@ -2136,10 +2137,10 @@
       <c r="U6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="V6" s="35" t="s">
+      <c r="V6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="W6" s="35"/>
+      <c r="W6" s="36"/>
       <c r="Y6" s="2" t="s">
         <v>33</v>
       </c>
@@ -2164,10 +2165,10 @@
       <c r="AG6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="AH6" s="35" t="s">
+      <c r="AH6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="AI6" s="35"/>
+      <c r="AI6" s="36"/>
       <c r="AK6" s="2" t="s">
         <v>33</v>
       </c>
@@ -2192,10 +2193,10 @@
       <c r="AS6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="AT6" s="35" t="s">
+      <c r="AT6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="AU6" s="35"/>
+      <c r="AU6" s="36"/>
       <c r="AW6" s="2" t="s">
         <v>33</v>
       </c>
@@ -2213,10 +2214,10 @@
       <c r="BE6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="BF6" s="35" t="s">
+      <c r="BF6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="BG6" s="35"/>
+      <c r="BG6" s="36"/>
     </row>
     <row r="7" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -4752,14 +4753,14 @@
       <c r="B32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="33">
+      <c r="C32" s="34">
         <f>C31+D31</f>
         <v>210</v>
       </c>
-      <c r="D32" s="33"/>
+      <c r="D32" s="34"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
     </row>
     <row r="33" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
@@ -4784,12 +4785,12 @@
     <row r="34" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="H34" s="33"/>
+      <c r="H34" s="34"/>
     </row>
     <row r="35" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="H35" s="33"/>
+      <c r="H35" s="34"/>
       <c r="R35" t="s">
         <v>33</v>
       </c>
@@ -4978,10 +4979,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC1E50C3-E510-44DF-9648-92EC3D48E3D3}">
-  <dimension ref="B2:BC41"/>
+  <dimension ref="B2:BC53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AS17" sqref="AS17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4995,12 +4996,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="C2" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="2:55" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
@@ -5011,12 +5012,12 @@
       </c>
     </row>
     <row r="4" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
       <c r="N4" s="27" t="s">
         <v>46</v>
       </c>
@@ -5060,14 +5061,14 @@
       <c r="BC4" s="27"/>
     </row>
     <row r="5" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="33">
+      <c r="B5" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="34">
         <v>2024</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33" t="s">
+      <c r="D5" s="34"/>
+      <c r="E5" s="34" t="s">
         <v>28</v>
       </c>
       <c r="H5" t="s">
@@ -5147,14 +5148,14 @@
       <c r="BC5" s="27"/>
     </row>
     <row r="6" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B6" s="33"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="33"/>
+      <c r="E6" s="34"/>
       <c r="H6" s="2" t="s">
         <v>33</v>
       </c>
@@ -5178,10 +5179,10 @@
       <c r="Q6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="35" t="s">
+      <c r="R6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="S6" s="35"/>
+      <c r="S6" s="36"/>
       <c r="U6" s="2" t="s">
         <v>33</v>
       </c>
@@ -5203,10 +5204,10 @@
       <c r="AC6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="AD6" s="35" t="s">
+      <c r="AD6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="AE6" s="35"/>
+      <c r="AE6" s="36"/>
       <c r="AG6" s="2" t="s">
         <v>33</v>
       </c>
@@ -5228,10 +5229,10 @@
       <c r="AO6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="AP6" s="35" t="s">
+      <c r="AP6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="AQ6" s="35"/>
+      <c r="AQ6" s="36"/>
       <c r="AS6" s="2" t="s">
         <v>33</v>
       </c>
@@ -5249,10 +5250,10 @@
       <c r="BA6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="BB6" s="35" t="s">
+      <c r="BB6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="BC6" s="35"/>
+      <c r="BC6" s="36"/>
     </row>
     <row r="7" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -7389,6 +7390,10 @@
         <f t="shared" ref="D31" si="10">SUM(D7:D30)</f>
         <v>202</v>
       </c>
+      <c r="E31">
+        <f>SUM(E7:E30)</f>
+        <v>210</v>
+      </c>
       <c r="S31" s="4">
         <f t="shared" ref="S31" si="11">SUM(S7:S30)</f>
         <v>202</v>
@@ -7402,11 +7407,11 @@
       <c r="B32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="33">
+      <c r="C32" s="34">
         <f>C31+D31</f>
         <v>210</v>
       </c>
-      <c r="D32" s="33"/>
+      <c r="D32" s="34"/>
     </row>
     <row r="33" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
@@ -7415,13 +7420,25 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="N33" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
+      </c>
+      <c r="O33" t="s">
+        <v>34</v>
+      </c>
+      <c r="P33" t="s">
+        <v>35</v>
       </c>
       <c r="Z33" s="3" t="s">
         <v>42</v>
       </c>
       <c r="AL33" s="3" t="s">
-        <v>42</v>
+        <v>33</v>
+      </c>
+      <c r="AM33" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN33" t="s">
+        <v>35</v>
       </c>
       <c r="AX33" s="3" t="s">
         <v>42</v>
@@ -7430,18 +7447,42 @@
     <row r="34" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
+      <c r="N34" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O34" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="P34" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL34" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM34" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="AN34" s="23" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="35" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="N35" t="s">
-        <v>33</v>
+      <c r="N35" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O35" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="Z35" t="s">
         <v>33</v>
       </c>
-      <c r="AL35" t="s">
-        <v>33</v>
+      <c r="AL35" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM35" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="AX35" t="s">
         <v>33</v>
@@ -7450,14 +7491,20 @@
     <row r="36" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="N36" t="s">
-        <v>34</v>
+      <c r="N36" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O36" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="Z36" t="s">
         <v>34</v>
       </c>
-      <c r="AL36" t="s">
-        <v>34</v>
+      <c r="AL36" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM36" s="12" t="s">
+        <v>15</v>
       </c>
       <c r="AX36" t="s">
         <v>34</v>
@@ -7466,14 +7513,17 @@
     <row r="37" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="N37" t="s">
-        <v>35</v>
+      <c r="N37" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="Z37" t="s">
         <v>35</v>
       </c>
-      <c r="AL37" t="s">
-        <v>35</v>
+      <c r="AL37" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM37" s="23" t="s">
+        <v>17</v>
       </c>
       <c r="AX37" t="s">
         <v>35</v>
@@ -7482,18 +7532,135 @@
     <row r="38" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
+      <c r="N38" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AL38" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AM38" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="39" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
+      <c r="N39" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL39" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM39" s="19" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="40" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
+      <c r="N40" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL40" s="12" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="41" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
+      <c r="N41" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="AL41" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N42" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL42" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N43" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL43" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N44" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL44" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N45" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL45" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N46" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL46" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N47" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AL47" s="19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N48" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL48" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="14:38" x14ac:dyDescent="0.25">
+      <c r="N49" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="AL49" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="14:38" x14ac:dyDescent="0.25">
+      <c r="N50" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL50" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="14:38" x14ac:dyDescent="0.25">
+      <c r="N51" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="14:38" x14ac:dyDescent="0.25">
+      <c r="N52" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="14:38" x14ac:dyDescent="0.25">
+      <c r="N53" s="12" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -7514,10 +7681,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A07BDC3-86C1-49BC-A7E6-7DF335B10BC5}">
-  <dimension ref="B2:BC41"/>
+  <dimension ref="B2:BC52"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ6" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="T4" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7532,12 +7699,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="C2" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="2:55" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
@@ -7548,12 +7715,12 @@
       </c>
     </row>
     <row r="4" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
       <c r="N4" s="27" t="s">
         <v>46</v>
       </c>
@@ -7589,14 +7756,14 @@
       <c r="BC4" s="27"/>
     </row>
     <row r="5" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="33">
+      <c r="B5" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="34">
         <v>2024</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33" t="s">
+      <c r="D5" s="34"/>
+      <c r="E5" s="34" t="s">
         <v>28</v>
       </c>
       <c r="H5" t="s">
@@ -7654,14 +7821,14 @@
       <c r="BC5" s="27"/>
     </row>
     <row r="6" spans="2:55" x14ac:dyDescent="0.25">
-      <c r="B6" s="33"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="33"/>
+      <c r="E6" s="34"/>
       <c r="H6" s="2" t="s">
         <v>33</v>
       </c>
@@ -7682,10 +7849,10 @@
       <c r="Q6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="R6" s="35" t="s">
+      <c r="R6" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="S6" s="35"/>
+      <c r="S6" s="30"/>
       <c r="U6" s="2" t="s">
         <v>33</v>
       </c>
@@ -7707,10 +7874,10 @@
       <c r="AC6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="AD6" s="35" t="s">
+      <c r="AD6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="AE6" s="35"/>
+      <c r="AE6" s="36"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="9"/>
       <c r="AI6" s="9"/>
@@ -7719,8 +7886,8 @@
       <c r="AM6" s="29"/>
       <c r="AN6" s="29"/>
       <c r="AO6" s="30"/>
-      <c r="AP6" s="35"/>
-      <c r="AQ6" s="35"/>
+      <c r="AP6" s="36"/>
+      <c r="AQ6" s="36"/>
       <c r="AS6" s="2"/>
       <c r="AU6" s="9"/>
       <c r="AV6" s="11"/>
@@ -7728,8 +7895,8 @@
       <c r="AY6" s="29"/>
       <c r="AZ6" s="29"/>
       <c r="BA6" s="30"/>
-      <c r="BB6" s="35"/>
-      <c r="BC6" s="35"/>
+      <c r="BB6" s="36"/>
+      <c r="BC6" s="36"/>
     </row>
     <row r="7" spans="2:55" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -7853,15 +8020,15 @@
         <v>5</v>
       </c>
       <c r="O8" s="13">
-        <f t="shared" ref="O8:O30" si="1">SQRT((C8 - $J$6)^2)</f>
+        <f t="shared" ref="O8:O29" si="1">SQRT((C8 - $J$6)^2)</f>
         <v>0</v>
       </c>
       <c r="P8" s="13">
-        <f t="shared" ref="P8:P30" si="2">SQRT((C8 - $J$7)^2)</f>
+        <f t="shared" ref="P8:P29" si="2">SQRT((C8 - $J$7)^2)</f>
         <v>1</v>
       </c>
       <c r="Q8" s="14">
-        <f t="shared" ref="Q8:Q30" si="3">SQRT((C8 - $J$8)^2)</f>
+        <f t="shared" ref="Q8:Q29" si="3">SQRT((C8 - $J$8)^2)</f>
         <v>3</v>
       </c>
       <c r="R8" s="11" t="s">
@@ -9431,7 +9598,7 @@
         <f t="shared" ref="S31" si="8">SUM(S7:S30)</f>
         <v>8</v>
       </c>
-      <c r="AE31" s="36">
+      <c r="AE31" s="33">
         <f t="shared" ref="AE31" si="9">SUM(AE7:AE30)</f>
         <v>0</v>
       </c>
@@ -9440,11 +9607,11 @@
       <c r="B32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="33">
+      <c r="C32" s="34">
         <f>C31+D31</f>
         <v>210</v>
       </c>
-      <c r="D32" s="33"/>
+      <c r="D32" s="34"/>
     </row>
     <row r="33" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
@@ -9453,67 +9620,146 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="N33" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z33" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="O33" t="s">
+        <v>34</v>
+      </c>
+      <c r="P33" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z33" s="3"/>
       <c r="AL33" s="3"/>
       <c r="AX33" s="3"/>
     </row>
     <row r="34" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
+      <c r="N34" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="O34" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="P34" s="19" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="35" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="N35" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z35" t="s">
-        <v>33</v>
+      <c r="N35" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O35" s="19" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="N36" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z36" t="s">
-        <v>34</v>
+      <c r="N36" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O36" s="19" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="N37" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z37" t="s">
-        <v>35</v>
+      <c r="N37" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="O37" s="12" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
+      <c r="N38" s="12" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="39" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
+      <c r="N39" s="23" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="40" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
+      <c r="N40" s="19" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="41" spans="3:50" x14ac:dyDescent="0.25">
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
+      <c r="N41" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N42" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N43" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N44" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N45" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N46" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N47" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="3:50" x14ac:dyDescent="0.25">
+      <c r="N48" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N49" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N50" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N51" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N52" s="12" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="AD6:AE6"/>
+  <mergeCells count="9">
     <mergeCell ref="AP6:AQ6"/>
     <mergeCell ref="BB6:BC6"/>
     <mergeCell ref="C32:D32"/>
@@ -9522,7 +9768,314 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="AD6:AE6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33A0F34F-35EB-4D62-B10C-97ED54243FFE}">
+  <dimension ref="B1:P16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+    </row>
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="H3" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="34">
+        <v>2024</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="34"/>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="34"/>
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="11"/>
+      <c r="N5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E16" si="0">SUM(C6:D6)</f>
+        <v>5</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2</v>
+      </c>
+      <c r="J6" s="7">
+        <v>1</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="12"/>
+      <c r="M6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+      <c r="J7" s="7">
+        <v>3</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update Revisi Bu Zahra Kirim Online Pertama
</commit_message>
<xml_diff>
--- a/Perhitungan K-Means K_3.xlsx
+++ b/Perhitungan K-Means K_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CADANGAN SKRIPSI GIT HUB\DATA SKRIPSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F1EA45-D239-4AB9-949B-6188FE6F5C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6747D75-2645-4C78-B9E5-940D6626E4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{204938CF-0984-440D-97FB-7D0080130912}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{204938CF-0984-440D-97FB-7D0080130912}"/>
   </bookViews>
   <sheets>
     <sheet name="Normalisasi" sheetId="1" r:id="rId1"/>
@@ -297,7 +297,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -806,6 +806,25 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="8" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -826,25 +845,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="8" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1179,53 +1179,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C2" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
+      <c r="C2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J3" s="64" t="s">
+      <c r="J3" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="63">
+      <c r="C5" s="70">
         <v>2021</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63">
+      <c r="D5" s="70"/>
+      <c r="E5" s="70">
         <v>2022</v>
       </c>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63" t="s">
+      <c r="F5" s="70"/>
+      <c r="G5" s="70" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="63" t="s">
+      <c r="J5" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="63">
+      <c r="K5" s="70">
         <v>2021</v>
       </c>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63">
+      <c r="L5" s="70"/>
+      <c r="M5" s="70">
         <v>2022</v>
       </c>
-      <c r="N5" s="63"/>
+      <c r="N5" s="70"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="63"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1238,8 +1238,8 @@
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="63"/>
-      <c r="J6" s="63"/>
+      <c r="G6" s="70"/>
+      <c r="J6" s="70"/>
       <c r="K6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2269,23 +2269,23 @@
       <c r="B32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="63">
+      <c r="C32" s="70">
         <f>C31+D31</f>
         <v>219</v>
       </c>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63">
+      <c r="D32" s="70"/>
+      <c r="E32" s="70">
         <f>E31+F31</f>
         <v>178</v>
       </c>
-      <c r="F32" s="63"/>
+      <c r="F32" s="70"/>
       <c r="J32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="63"/>
+      <c r="K32" s="70"/>
+      <c r="L32" s="70"/>
+      <c r="M32" s="70"/>
+      <c r="N32" s="70"/>
     </row>
     <row r="33" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
@@ -2347,11 +2347,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:L5"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="G5:G6"/>
@@ -2360,6 +2355,11 @@
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="K32:L32"/>
     <mergeCell ref="M32:N32"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2387,19 +2387,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="C2" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
+      <c r="C2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
     </row>
     <row r="3" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="H3" s="64" t="s">
+      <c r="H3" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
       <c r="L3" t="s">
         <v>31</v>
       </c>
@@ -2408,12 +2408,12 @@
       </c>
     </row>
     <row r="4" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="L4" s="64" t="s">
+      <c r="L4" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
+      <c r="M4" s="71"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="71"/>
       <c r="R4" s="27" t="s">
         <v>46</v>
       </c>
@@ -2457,14 +2457,14 @@
       <c r="BG4" s="27"/>
     </row>
     <row r="5" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="63">
+      <c r="C5" s="70">
         <v>2024</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63" t="s">
+      <c r="D5" s="70"/>
+      <c r="E5" s="70" t="s">
         <v>28</v>
       </c>
       <c r="H5" s="4"/>
@@ -2547,14 +2547,14 @@
       <c r="BG5" s="27"/>
     </row>
     <row r="6" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="B6" s="63"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="63"/>
+      <c r="E6" s="70"/>
       <c r="H6" s="4" t="s">
         <v>1</v>
       </c>
@@ -2591,10 +2591,10 @@
       <c r="U6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="V6" s="65" t="s">
+      <c r="V6" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="W6" s="65"/>
+      <c r="W6" s="72"/>
       <c r="Y6" s="2" t="s">
         <v>33</v>
       </c>
@@ -2619,10 +2619,10 @@
       <c r="AG6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="AH6" s="65" t="s">
+      <c r="AH6" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="AI6" s="65"/>
+      <c r="AI6" s="72"/>
       <c r="AK6" s="2" t="s">
         <v>33</v>
       </c>
@@ -2647,10 +2647,10 @@
       <c r="AS6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="AT6" s="65" t="s">
+      <c r="AT6" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="AU6" s="65"/>
+      <c r="AU6" s="72"/>
       <c r="AW6" s="2" t="s">
         <v>33</v>
       </c>
@@ -2668,10 +2668,10 @@
       <c r="BE6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="BF6" s="65" t="s">
+      <c r="BF6" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="BG6" s="65"/>
+      <c r="BG6" s="72"/>
     </row>
     <row r="7" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -5207,14 +5207,14 @@
       <c r="B32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="63">
+      <c r="C32" s="70">
         <f>C31+D31</f>
         <v>210</v>
       </c>
-      <c r="D32" s="63"/>
+      <c r="D32" s="70"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="63"/>
+      <c r="I32" s="70"/>
+      <c r="J32" s="70"/>
     </row>
     <row r="33" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
@@ -5239,12 +5239,12 @@
     <row r="34" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="H34" s="63"/>
+      <c r="H34" s="70"/>
     </row>
     <row r="35" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="H35" s="63"/>
+      <c r="H35" s="70"/>
       <c r="R35" t="s">
         <v>33</v>
       </c>
@@ -5411,6 +5411,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="V6:W6"/>
     <mergeCell ref="AH6:AI6"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="I32:J32"/>
@@ -5419,11 +5424,6 @@
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="AT6:AU6"/>
     <mergeCell ref="L4:O4"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="V6:W6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5442,12 +5442,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
+      <c r="C1" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
@@ -5458,22 +5458,22 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H3" s="64" t="s">
+      <c r="H3" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="63">
+      <c r="C4" s="70">
         <v>2024</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63" t="s">
+      <c r="D4" s="70"/>
+      <c r="E4" s="70" t="s">
         <v>28</v>
       </c>
       <c r="H4" t="s">
@@ -5493,14 +5493,14 @@
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="63"/>
+      <c r="B5" s="70"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="63"/>
+      <c r="E5" s="70"/>
       <c r="H5" s="2" t="s">
         <v>33</v>
       </c>
@@ -5742,8 +5742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7247C1F-547F-40E3-8593-729479C08754}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5752,7 +5752,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="73" t="s">
         <v>57</v>
       </c>
       <c r="B1" s="45">
@@ -5769,7 +5769,7 @@
       <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67"/>
+      <c r="A2" s="74"/>
       <c r="B2" s="48" t="s">
         <v>58</v>
       </c>
@@ -5790,7 +5790,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68"/>
+      <c r="A3" s="75"/>
       <c r="B3" s="51" t="s">
         <v>59</v>
       </c>
@@ -6473,8 +6473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC1E50C3-E510-44DF-9648-92EC3D48E3D3}">
   <dimension ref="A2:BM61"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6489,9 +6489,9 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
       <c r="K2" s="38"/>
       <c r="W2" s="38"/>
       <c r="AQ2" s="38"/>
@@ -6552,12 +6552,12 @@
       <c r="BM3" s="38"/>
     </row>
     <row r="4" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
       <c r="K4" s="38"/>
       <c r="M4" s="27" t="s">
         <v>46</v>
@@ -6615,13 +6615,13 @@
       <c r="BM4" s="38"/>
     </row>
     <row r="5" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="70" t="s">
         <v>81</v>
       </c>
       <c r="E5" t="s">
@@ -6706,9 +6706,9 @@
       <c r="BM5" s="38"/>
     </row>
     <row r="6" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
       <c r="G6" s="2" t="s">
         <v>33</v>
       </c>
@@ -6797,8 +6797,8 @@
       <c r="AX6" s="35"/>
       <c r="AY6" s="35"/>
       <c r="AZ6" s="36"/>
-      <c r="BA6" s="69"/>
-      <c r="BB6" s="69"/>
+      <c r="BA6" s="76"/>
+      <c r="BB6" s="76"/>
       <c r="BC6" s="38"/>
       <c r="BD6" s="38"/>
       <c r="BE6" s="38"/>
@@ -7631,7 +7631,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G14" s="75">
+      <c r="G14" s="68">
         <f>G13/23</f>
         <v>8.8131609870740299E-2</v>
       </c>
@@ -10878,8 +10878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A07BDC3-86C1-49BC-A7E6-7DF335B10BC5}">
   <dimension ref="B2:BB54"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10893,11 +10893,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="C2" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
+      <c r="C2" s="71" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
     </row>
     <row r="3" spans="2:54" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
@@ -10923,12 +10923,12 @@
       <c r="AV3" s="38"/>
     </row>
     <row r="4" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="G4" s="64" t="s">
+      <c r="G4" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
       <c r="M4" s="27" t="s">
         <v>46</v>
       </c>
@@ -10972,13 +10972,13 @@
       <c r="BB4" s="27"/>
     </row>
     <row r="5" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="70" t="s">
         <v>81</v>
       </c>
       <c r="E5" t="s">
@@ -11044,9 +11044,9 @@
       <c r="BB5" s="27"/>
     </row>
     <row r="6" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
       <c r="G6" s="2" t="s">
         <v>33</v>
       </c>
@@ -11105,8 +11105,8 @@
       <c r="AL6" s="35"/>
       <c r="AM6" s="35"/>
       <c r="AN6" s="36"/>
-      <c r="AO6" s="69"/>
-      <c r="AP6" s="69"/>
+      <c r="AO6" s="76"/>
+      <c r="AP6" s="76"/>
       <c r="AQ6" s="38"/>
       <c r="AR6" s="32"/>
       <c r="AS6" s="38"/>
@@ -11117,8 +11117,8 @@
       <c r="AX6" s="29"/>
       <c r="AY6" s="29"/>
       <c r="AZ6" s="30"/>
-      <c r="BA6" s="65"/>
-      <c r="BB6" s="65"/>
+      <c r="BA6" s="72"/>
+      <c r="BB6" s="72"/>
     </row>
     <row r="7" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
@@ -13611,13 +13611,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G4:J4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="AO6:AP6"/>
     <mergeCell ref="BA6:BB6"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="G4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13627,7 +13627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF750BB8-12B1-4DDA-A3C7-AD936B93E529}">
   <dimension ref="A3:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:F28"/>
     </sheetView>
   </sheetViews>
@@ -13638,502 +13638,502 @@
   <sheetData>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="71" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="71" t="s">
+      <c r="C4" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="71" t="s">
+      <c r="E4" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="72" t="s">
+      <c r="F4" s="65" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="76">
+      <c r="B5" s="69">
         <v>0.04</v>
       </c>
-      <c r="C5" s="76">
+      <c r="C5" s="69">
         <v>0.01</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="69">
         <v>0.17</v>
       </c>
-      <c r="E5" s="76">
+      <c r="E5" s="69">
         <v>0.96</v>
       </c>
-      <c r="F5" s="74" t="s">
+      <c r="F5" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="76">
+      <c r="B6" s="69">
         <v>0.06</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="69">
         <v>0.03</v>
       </c>
-      <c r="D6" s="76">
+      <c r="D6" s="69">
         <v>0.15</v>
       </c>
-      <c r="E6" s="76">
+      <c r="E6" s="69">
         <v>0.94</v>
       </c>
-      <c r="F6" s="74" t="s">
+      <c r="F6" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="76">
+      <c r="B7" s="69">
         <v>0.1</v>
       </c>
-      <c r="C7" s="76">
+      <c r="C7" s="69">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="69">
         <v>0.11</v>
       </c>
-      <c r="E7" s="76">
+      <c r="E7" s="69">
         <v>0.9</v>
       </c>
-      <c r="F7" s="74" t="s">
+      <c r="F7" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="76">
+      <c r="B8" s="69">
         <v>0.3</v>
       </c>
-      <c r="C8" s="76">
+      <c r="C8" s="69">
         <v>0.27</v>
       </c>
-      <c r="D8" s="76">
+      <c r="D8" s="69">
         <v>0.09</v>
       </c>
-      <c r="E8" s="76">
+      <c r="E8" s="69">
         <v>0.7</v>
       </c>
-      <c r="F8" s="74" t="s">
+      <c r="F8" s="67" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="76">
+      <c r="B9" s="69">
         <v>0.03</v>
       </c>
-      <c r="C9" s="76">
-        <v>0</v>
-      </c>
-      <c r="D9" s="76">
+      <c r="C9" s="69">
+        <v>0</v>
+      </c>
+      <c r="D9" s="69">
         <v>0.18</v>
       </c>
-      <c r="E9" s="76">
+      <c r="E9" s="69">
         <v>0.97</v>
       </c>
-      <c r="F9" s="74" t="s">
+      <c r="F9" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="76">
+      <c r="B10" s="69">
         <v>0.21</v>
       </c>
-      <c r="C10" s="76">
+      <c r="C10" s="69">
         <v>0.18</v>
       </c>
-      <c r="D10" s="76">
-        <v>0</v>
-      </c>
-      <c r="E10" s="76">
+      <c r="D10" s="69">
+        <v>0</v>
+      </c>
+      <c r="E10" s="69">
         <v>0.79</v>
       </c>
-      <c r="F10" s="74" t="s">
+      <c r="F10" s="67" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="76">
+      <c r="B11" s="69">
         <v>0.05</v>
       </c>
-      <c r="C11" s="76">
+      <c r="C11" s="69">
         <v>0.02</v>
       </c>
-      <c r="D11" s="76">
+      <c r="D11" s="69">
         <v>0.16</v>
       </c>
-      <c r="E11" s="76">
+      <c r="E11" s="69">
         <v>0.95</v>
       </c>
-      <c r="F11" s="74" t="s">
+      <c r="F11" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="76">
+      <c r="B12" s="69">
         <v>1</v>
       </c>
-      <c r="C12" s="76">
+      <c r="C12" s="69">
         <v>0.97</v>
       </c>
-      <c r="D12" s="76">
+      <c r="D12" s="69">
         <v>0.79</v>
       </c>
-      <c r="E12" s="76">
-        <v>0</v>
-      </c>
-      <c r="F12" s="74" t="s">
+      <c r="E12" s="69">
+        <v>0</v>
+      </c>
+      <c r="F12" s="67" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="76">
+      <c r="B13" s="69">
         <v>0.15</v>
       </c>
-      <c r="C13" s="76">
+      <c r="C13" s="69">
         <v>0.12</v>
       </c>
-      <c r="D13" s="76">
+      <c r="D13" s="69">
         <v>0.06</v>
       </c>
-      <c r="E13" s="76">
+      <c r="E13" s="69">
         <v>0.85</v>
       </c>
-      <c r="F13" s="74" t="s">
+      <c r="F13" s="67" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="76">
+      <c r="B14" s="69">
         <v>0.05</v>
       </c>
-      <c r="C14" s="76">
+      <c r="C14" s="69">
         <v>0.02</v>
       </c>
-      <c r="D14" s="76">
+      <c r="D14" s="69">
         <v>0.16</v>
       </c>
-      <c r="E14" s="76">
+      <c r="E14" s="69">
         <v>0.95</v>
       </c>
-      <c r="F14" s="74" t="s">
+      <c r="F14" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="76">
+      <c r="B15" s="69">
         <v>0.01</v>
       </c>
-      <c r="C15" s="76">
+      <c r="C15" s="69">
         <v>0.02</v>
       </c>
-      <c r="D15" s="76">
+      <c r="D15" s="69">
         <v>0.2</v>
       </c>
-      <c r="E15" s="76">
+      <c r="E15" s="69">
         <v>0.99</v>
       </c>
-      <c r="F15" s="74" t="s">
+      <c r="F15" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="73" t="s">
+      <c r="A16" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="76">
+      <c r="B16" s="69">
         <v>0.16</v>
       </c>
-      <c r="C16" s="76">
+      <c r="C16" s="69">
         <v>0.13</v>
       </c>
-      <c r="D16" s="76">
+      <c r="D16" s="69">
         <v>0.05</v>
       </c>
-      <c r="E16" s="76">
+      <c r="E16" s="69">
         <v>0.84</v>
       </c>
-      <c r="F16" s="74" t="s">
+      <c r="F16" s="67" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="76">
-        <v>0</v>
-      </c>
-      <c r="C17" s="76">
+      <c r="B17" s="69">
+        <v>0</v>
+      </c>
+      <c r="C17" s="69">
         <v>0.03</v>
       </c>
-      <c r="D17" s="76">
+      <c r="D17" s="69">
         <v>0.21</v>
       </c>
-      <c r="E17" s="76">
+      <c r="E17" s="69">
         <v>1</v>
       </c>
-      <c r="F17" s="74" t="s">
+      <c r="F17" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="76">
+      <c r="B18" s="69">
         <v>0.24</v>
       </c>
-      <c r="C18" s="76">
+      <c r="C18" s="69">
         <v>0.21</v>
       </c>
-      <c r="D18" s="76">
+      <c r="D18" s="69">
         <v>0.03</v>
       </c>
-      <c r="E18" s="76">
+      <c r="E18" s="69">
         <v>0.76</v>
       </c>
-      <c r="F18" s="74" t="s">
+      <c r="F18" s="67" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="76">
+      <c r="B19" s="69">
         <v>0.27</v>
       </c>
-      <c r="C19" s="76">
+      <c r="C19" s="69">
         <v>0.24</v>
       </c>
-      <c r="D19" s="76">
+      <c r="D19" s="69">
         <v>0.06</v>
       </c>
-      <c r="E19" s="76">
+      <c r="E19" s="69">
         <v>0.73</v>
       </c>
-      <c r="F19" s="74" t="s">
+      <c r="F19" s="67" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="73" t="s">
+      <c r="A20" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="76">
+      <c r="B20" s="69">
         <v>0.05</v>
       </c>
-      <c r="C20" s="76">
+      <c r="C20" s="69">
         <v>0.02</v>
       </c>
-      <c r="D20" s="76">
+      <c r="D20" s="69">
         <v>0.16</v>
       </c>
-      <c r="E20" s="76">
+      <c r="E20" s="69">
         <v>0.95</v>
       </c>
-      <c r="F20" s="74" t="s">
+      <c r="F20" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="76">
+      <c r="B21" s="69">
         <v>0.15</v>
       </c>
-      <c r="C21" s="76">
+      <c r="C21" s="69">
         <v>0.12</v>
       </c>
-      <c r="D21" s="76">
+      <c r="D21" s="69">
         <v>0.06</v>
       </c>
-      <c r="E21" s="76">
+      <c r="E21" s="69">
         <v>0.85</v>
       </c>
-      <c r="F21" s="74" t="s">
+      <c r="F21" s="67" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="73" t="s">
+      <c r="A22" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="76">
+      <c r="B22" s="69">
         <v>0.01</v>
       </c>
-      <c r="C22" s="76">
+      <c r="C22" s="69">
         <v>0.02</v>
       </c>
-      <c r="D22" s="76">
+      <c r="D22" s="69">
         <v>0.2</v>
       </c>
-      <c r="E22" s="76">
+      <c r="E22" s="69">
         <v>0.99</v>
       </c>
-      <c r="F22" s="74" t="s">
+      <c r="F22" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="76">
+      <c r="B23" s="69">
         <v>0.01</v>
       </c>
-      <c r="C23" s="76">
+      <c r="C23" s="69">
         <v>0.02</v>
       </c>
-      <c r="D23" s="76">
+      <c r="D23" s="69">
         <v>0.2</v>
       </c>
-      <c r="E23" s="76">
+      <c r="E23" s="69">
         <v>0.99</v>
       </c>
-      <c r="F23" s="74" t="s">
+      <c r="F23" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="73" t="s">
+      <c r="A24" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="76">
+      <c r="B24" s="69">
         <v>0.04</v>
       </c>
-      <c r="C24" s="76">
+      <c r="C24" s="69">
         <v>0.01</v>
       </c>
-      <c r="D24" s="76">
+      <c r="D24" s="69">
         <v>0.17</v>
       </c>
-      <c r="E24" s="76">
+      <c r="E24" s="69">
         <v>0.96</v>
       </c>
-      <c r="F24" s="74" t="s">
+      <c r="F24" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="73" t="s">
+      <c r="A25" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="76">
+      <c r="B25" s="69">
         <v>0.01</v>
       </c>
-      <c r="C25" s="76">
+      <c r="C25" s="69">
         <v>0.02</v>
       </c>
-      <c r="D25" s="76">
+      <c r="D25" s="69">
         <v>0.2</v>
       </c>
-      <c r="E25" s="76">
+      <c r="E25" s="69">
         <v>0.99</v>
       </c>
-      <c r="F25" s="74" t="s">
+      <c r="F25" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="73" t="s">
+      <c r="A26" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="76">
+      <c r="B26" s="69">
         <v>0.02</v>
       </c>
-      <c r="C26" s="76">
+      <c r="C26" s="69">
         <v>0.01</v>
       </c>
-      <c r="D26" s="76">
+      <c r="D26" s="69">
         <v>0.19</v>
       </c>
-      <c r="E26" s="76">
+      <c r="E26" s="69">
         <v>0.98</v>
       </c>
-      <c r="F26" s="74" t="s">
+      <c r="F26" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="73" t="s">
+      <c r="A27" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="76">
+      <c r="B27" s="69">
         <v>0.06</v>
       </c>
-      <c r="C27" s="76">
+      <c r="C27" s="69">
         <v>0.03</v>
       </c>
-      <c r="D27" s="76">
+      <c r="D27" s="69">
         <v>0.15</v>
       </c>
-      <c r="E27" s="76">
+      <c r="E27" s="69">
         <v>0.94</v>
       </c>
-      <c r="F27" s="74" t="s">
+      <c r="F27" s="67" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="73" t="s">
+      <c r="A28" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="76">
+      <c r="B28" s="69">
         <v>0.01</v>
       </c>
-      <c r="C28" s="76">
+      <c r="C28" s="69">
         <v>0.02</v>
       </c>
-      <c r="D28" s="76">
+      <c r="D28" s="69">
         <v>0.2</v>
       </c>
-      <c r="E28" s="76">
+      <c r="E28" s="69">
         <v>0.99</v>
       </c>
-      <c r="F28" s="74" t="s">
+      <c r="F28" s="67" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revisi Bu Bitari PART 2 pengujian metode
</commit_message>
<xml_diff>
--- a/Perhitungan K-Means K_3.xlsx
+++ b/Perhitungan K-Means K_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CADANGAN SKRIPSI GIT HUB\DATA SKRIPSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6747D75-2645-4C78-B9E5-940D6626E4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E536D8-FD03-4137-BD36-23C4E8E141CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{204938CF-0984-440D-97FB-7D0080130912}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{204938CF-0984-440D-97FB-7D0080130912}"/>
   </bookViews>
   <sheets>
     <sheet name="Normalisasi" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="89">
   <si>
     <t>DATA CURAS DAN CURANMOR KAB PROBOLINGGO 2021 - 2022</t>
   </si>
@@ -289,6 +289,15 @@
   </si>
   <si>
     <t>Krejengan</t>
+  </si>
+  <si>
+    <t>POLSEK SUMBERASIH</t>
+  </si>
+  <si>
+    <t>POLSEK TONGAS</t>
+  </si>
+  <si>
+    <t>POLSEK WONOMERTO</t>
   </si>
 </sst>
 </file>
@@ -648,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -845,6 +854,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2347,6 +2365,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="G5:G6"/>
@@ -2355,11 +2378,6 @@
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="K32:L32"/>
     <mergeCell ref="M32:N32"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5411,11 +5429,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="V6:W6"/>
     <mergeCell ref="AH6:AI6"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="I32:J32"/>
@@ -5424,6 +5437,11 @@
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="AT6:AU6"/>
     <mergeCell ref="L4:O4"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="V6:W6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5740,29 +5758,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7247C1F-547F-40E3-8593-729479C08754}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="45">
-        <v>2024</v>
+      <c r="B1" s="46">
+        <v>2022</v>
       </c>
       <c r="C1" s="46">
         <v>2023</v>
       </c>
-      <c r="D1" s="46">
-        <v>2022</v>
+      <c r="D1" s="45">
+        <v>2024</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>57</v>
       </c>
       <c r="H1" s="47"/>
       <c r="I1" s="47"/>
@@ -5770,15 +5792,16 @@
     </row>
     <row r="2" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="74"/>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="49" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="48" t="s">
         <v>58</v>
       </c>
+      <c r="G2" s="74"/>
       <c r="H2" s="50" t="s">
         <v>56</v>
       </c>
@@ -5791,15 +5814,16 @@
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="75"/>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="51" t="s">
         <v>59</v>
       </c>
+      <c r="G3" s="75"/>
       <c r="H3" s="52" t="s">
         <v>59</v>
       </c>
@@ -5810,518 +5834,569 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="54">
+        <v>62</v>
+      </c>
+      <c r="B4" s="55">
+        <v>4</v>
+      </c>
+      <c r="C4" s="55">
+        <v>2</v>
+      </c>
+      <c r="D4" s="54">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <f>D4+C4+B4</f>
+        <v>11</v>
+      </c>
+      <c r="G4" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="55">
+        <v>0</v>
+      </c>
+      <c r="I4" s="55">
+        <v>0</v>
+      </c>
+      <c r="J4" s="55">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f>J4+I4+H4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="55">
+        <v>2</v>
+      </c>
+      <c r="C5" s="55">
+        <v>8</v>
+      </c>
+      <c r="D5" s="54">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f>D5+C5+B5</f>
+        <v>14</v>
+      </c>
+      <c r="G5" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="55">
         <v>1</v>
       </c>
-      <c r="C4" s="55">
-        <v>0</v>
-      </c>
-      <c r="D4" s="55">
+      <c r="I5" s="55">
+        <v>0</v>
+      </c>
+      <c r="J5" s="55">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f>J5+I5+H5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="55">
+        <v>15</v>
+      </c>
+      <c r="C6" s="55">
+        <v>4</v>
+      </c>
+      <c r="D6" s="54">
         <v>2</v>
       </c>
-      <c r="E4">
-        <f>B4+C4+D4</f>
-        <v>3</v>
-      </c>
-      <c r="H4" s="55">
-        <v>0</v>
-      </c>
-      <c r="I4" s="55">
-        <v>0</v>
-      </c>
-      <c r="J4" s="55">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <f>H4+I4+J4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="54">
-        <v>0</v>
-      </c>
-      <c r="C5" s="55">
-        <v>4</v>
-      </c>
-      <c r="D5" s="55">
+      <c r="E6">
+        <f>D6+C6+B6</f>
+        <v>21</v>
+      </c>
+      <c r="G6" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="55">
         <v>1</v>
       </c>
-      <c r="E5">
-        <f t="shared" ref="E5:E23" si="0">B5+C5+D5</f>
-        <v>5</v>
-      </c>
-      <c r="H5" s="55">
-        <v>0</v>
-      </c>
-      <c r="I5" s="55">
-        <v>0</v>
-      </c>
-      <c r="J5" s="55">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <f t="shared" ref="K5:K24" si="1">H5+I5+J5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="53" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="54">
-        <v>5</v>
-      </c>
-      <c r="C6" s="55">
+      <c r="I6" s="55">
+        <v>1</v>
+      </c>
+      <c r="J6" s="55">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f>J6+I6+H6</f>
         <v>2</v>
-      </c>
-      <c r="D6" s="55">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="H6" s="55">
-        <v>0</v>
-      </c>
-      <c r="I6" s="55">
-        <v>0</v>
-      </c>
-      <c r="J6" s="55">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="53" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="54">
-        <v>2</v>
+        <v>68</v>
+      </c>
+      <c r="B7" s="55">
+        <v>11</v>
       </c>
       <c r="C7" s="55">
+        <v>26</v>
+      </c>
+      <c r="D7" s="54">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <f>D7+C7+B7</f>
+        <v>59</v>
+      </c>
+      <c r="G7" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="55">
         <v>1</v>
       </c>
-      <c r="D7" s="55">
+      <c r="I7" s="55">
+        <v>0</v>
+      </c>
+      <c r="J7" s="55">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f>J7+I7+H7</f>
         <v>1</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H7" s="55">
-        <v>0</v>
-      </c>
-      <c r="I7" s="55">
-        <v>0</v>
-      </c>
-      <c r="J7" s="55">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="53" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="54">
+        <v>74</v>
+      </c>
+      <c r="B8" s="55">
+        <v>3</v>
+      </c>
+      <c r="C8" s="55">
         <v>1</v>
       </c>
-      <c r="C8" s="55">
-        <v>2</v>
-      </c>
-      <c r="D8" s="55">
+      <c r="D8" s="54">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <f>D8+C8+B8</f>
+        <v>8</v>
+      </c>
+      <c r="G8" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="55">
+        <v>0</v>
+      </c>
+      <c r="I8" s="55">
+        <v>0</v>
+      </c>
+      <c r="J8" s="55">
         <v>1</v>
       </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H8" s="55">
-        <v>0</v>
-      </c>
-      <c r="I8" s="55">
-        <v>0</v>
-      </c>
-      <c r="J8" s="55">
-        <v>0</v>
-      </c>
       <c r="K8">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>J8+I8+H8</f>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="B9" s="54">
+        <v>70</v>
+      </c>
+      <c r="B9" s="55">
+        <v>7</v>
+      </c>
+      <c r="C9" s="55">
+        <v>17</v>
+      </c>
+      <c r="D9" s="54">
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <f>D9+C9+B9</f>
+        <v>42</v>
+      </c>
+      <c r="G9" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="55">
+        <v>0</v>
+      </c>
+      <c r="I9" s="55">
+        <v>0</v>
+      </c>
+      <c r="J9" s="55">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f>J9+I9+H9</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="55">
+        <v>10</v>
+      </c>
+      <c r="C10" s="55">
+        <v>3</v>
+      </c>
+      <c r="D10" s="54">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>D10+C10+B10</f>
         <v>13</v>
       </c>
-      <c r="C9" s="55">
-        <v>16</v>
-      </c>
-      <c r="D9" s="55">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="H9" s="55">
-        <v>0</v>
-      </c>
-      <c r="I9" s="55">
-        <v>0</v>
-      </c>
-      <c r="J9" s="55">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="54">
+      <c r="G10" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="55">
+        <v>0</v>
+      </c>
+      <c r="I10" s="55">
+        <v>0</v>
+      </c>
+      <c r="J10" s="55">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f>J10+I10+H10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="55">
+        <v>100</v>
+      </c>
+      <c r="C11" s="55">
+        <v>51</v>
+      </c>
+      <c r="D11" s="54">
+        <v>37</v>
+      </c>
+      <c r="E11">
+        <f>D11+C11+B11</f>
+        <v>188</v>
+      </c>
+      <c r="G11" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="55">
+        <v>0</v>
+      </c>
+      <c r="I11" s="55">
         <v>1</v>
       </c>
-      <c r="C10" s="55">
-        <v>1</v>
-      </c>
-      <c r="D10" s="55">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H10" s="55">
-        <v>0</v>
-      </c>
-      <c r="I10" s="55">
-        <v>0</v>
-      </c>
-      <c r="J10" s="55">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="54">
-        <v>4</v>
-      </c>
-      <c r="C11" s="55">
-        <v>8</v>
-      </c>
-      <c r="D11" s="55">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="H11" s="55">
-        <v>0</v>
-      </c>
-      <c r="I11" s="55">
-        <v>0</v>
-      </c>
       <c r="J11" s="55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
+        <f>J11+I11+H11</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="54">
-        <v>22</v>
+        <v>75</v>
+      </c>
+      <c r="B12" s="55">
+        <v>20</v>
       </c>
       <c r="C12" s="55">
-        <v>26</v>
-      </c>
-      <c r="D12" s="55">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="D12" s="54">
+        <v>9</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>59</v>
+        <f>D12+C12+B12</f>
+        <v>30</v>
+      </c>
+      <c r="G12" s="53" t="s">
+        <v>75</v>
       </c>
       <c r="H12" s="55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="55">
         <v>0</v>
       </c>
       <c r="J12" s="55">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f>J12+I12+H12</f>
         <v>1</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="1"/>
+    </row>
+    <row r="13" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="58">
+        <v>2</v>
+      </c>
+      <c r="C13" s="58">
+        <v>8</v>
+      </c>
+      <c r="D13" s="57">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <f>D13+C13+B13</f>
+        <v>13</v>
+      </c>
+      <c r="G13" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="H13" s="58">
+        <v>0</v>
+      </c>
+      <c r="I13" s="58">
+        <v>0</v>
+      </c>
+      <c r="J13" s="58">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f>J13+I13+H13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="55">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="54">
-        <v>21</v>
-      </c>
-      <c r="C13" s="55">
-        <v>10</v>
-      </c>
-      <c r="D13" s="55">
-        <v>17</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="H13" s="55">
-        <v>0</v>
-      </c>
-      <c r="I13" s="55">
-        <v>0</v>
-      </c>
-      <c r="J13" s="55">
-        <v>0</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="53" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="54">
-        <v>18</v>
-      </c>
       <c r="C14" s="55">
-        <v>17</v>
-      </c>
-      <c r="D14" s="55">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="D14" s="54">
+        <v>2</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <f>D14+C14+B14</f>
+        <v>4</v>
+      </c>
+      <c r="G14" s="53" t="s">
+        <v>63</v>
       </c>
       <c r="H14" s="55">
+        <v>0</v>
+      </c>
+      <c r="I14" s="55">
+        <v>0</v>
+      </c>
+      <c r="J14" s="55">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f>J14+I14+H14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="55">
+        <v>4</v>
+      </c>
+      <c r="C15" s="55">
+        <v>16</v>
+      </c>
+      <c r="D15" s="54">
+        <v>13</v>
+      </c>
+      <c r="E15">
+        <f>D15+C15+B15</f>
+        <v>33</v>
+      </c>
+      <c r="G15" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="55">
+        <v>0</v>
+      </c>
+      <c r="I15" s="55">
+        <v>0</v>
+      </c>
+      <c r="J15" s="55">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f>J15+I15+H15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="55">
+        <v>2</v>
+      </c>
+      <c r="C16" s="55">
+        <v>0</v>
+      </c>
+      <c r="D16" s="54">
         <v>1</v>
       </c>
-      <c r="I14" s="55">
-        <v>0</v>
-      </c>
-      <c r="J14" s="55">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="54">
-        <v>10</v>
-      </c>
-      <c r="C15" s="55">
-        <v>12</v>
-      </c>
-      <c r="D15" s="55">
-        <v>8</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="H15" s="55">
-        <v>0</v>
-      </c>
-      <c r="I15" s="55">
-        <v>0</v>
-      </c>
-      <c r="J15" s="55">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="54">
-        <v>37</v>
-      </c>
-      <c r="C16" s="55">
-        <v>51</v>
-      </c>
-      <c r="D16" s="55">
-        <v>100</v>
-      </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>188</v>
+        <f>D16+C16+B16</f>
+        <v>3</v>
+      </c>
+      <c r="G16" s="53" t="s">
+        <v>60</v>
       </c>
       <c r="H16" s="55">
         <v>0</v>
       </c>
       <c r="I16" s="55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="55">
         <v>0</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>J16+I16+H16</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="53" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="54">
-        <v>2</v>
+        <v>69</v>
+      </c>
+      <c r="B17" s="55">
+        <v>17</v>
       </c>
       <c r="C17" s="55">
-        <v>4</v>
-      </c>
-      <c r="D17" s="55">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="D17" s="54">
+        <v>21</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <f>D17+C17+B17</f>
+        <v>48</v>
+      </c>
+      <c r="G17" s="53" t="s">
+        <v>69</v>
       </c>
       <c r="H17" s="55">
         <v>0</v>
       </c>
       <c r="I17" s="55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f>J17+I17+H17</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="53" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="54">
+        <v>77</v>
+      </c>
+      <c r="B18" s="55">
+        <v>14</v>
+      </c>
+      <c r="C18" s="55">
+        <v>25</v>
+      </c>
+      <c r="D18" s="54">
+        <v>14</v>
+      </c>
+      <c r="E18">
+        <f>D18+C18+B18</f>
+        <v>53</v>
+      </c>
+      <c r="G18" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="55">
+        <v>0</v>
+      </c>
+      <c r="I18" s="55">
+        <v>1</v>
+      </c>
+      <c r="J18" s="55">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <f>J18+I18+H18</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="55">
         <v>4</v>
       </c>
-      <c r="C18" s="55">
-        <v>1</v>
-      </c>
-      <c r="D18" s="55">
-        <v>3</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
+      <c r="C19" s="55">
+        <v>4</v>
+      </c>
+      <c r="D19" s="54">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <f>D19+C19+B19</f>
+        <v>12</v>
+      </c>
+      <c r="G19" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="55">
+        <v>0</v>
+      </c>
+      <c r="I19" s="55">
+        <v>0</v>
+      </c>
+      <c r="J19" s="55">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <f>J19+I19+H19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="55">
         <v>8</v>
       </c>
-      <c r="H18" s="55">
-        <v>1</v>
-      </c>
-      <c r="I18" s="55">
-        <v>0</v>
-      </c>
-      <c r="J18" s="55">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="54">
-        <v>9</v>
-      </c>
-      <c r="C19" s="55">
-        <v>1</v>
-      </c>
-      <c r="D19" s="55">
-        <v>20</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
+      <c r="C20" s="55">
+        <v>12</v>
+      </c>
+      <c r="D20" s="54">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <f>D20+C20+B20</f>
         <v>30</v>
       </c>
-      <c r="H19" s="55">
-        <v>0</v>
-      </c>
-      <c r="I19" s="55">
-        <v>0</v>
-      </c>
-      <c r="J19" s="55">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="53" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="54">
-        <v>0</v>
-      </c>
-      <c r="C20" s="55">
-        <v>3</v>
-      </c>
-      <c r="D20" s="55">
-        <v>10</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>13</v>
+      <c r="G20" s="53" t="s">
+        <v>71</v>
       </c>
       <c r="H20" s="55">
         <v>0</v>
@@ -6333,137 +6408,252 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
+        <f>J20+I20+H20</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="53" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" s="54">
-        <v>14</v>
+        <v>61</v>
+      </c>
+      <c r="B21" s="55">
+        <v>1</v>
       </c>
       <c r="C21" s="55">
-        <v>25</v>
-      </c>
-      <c r="D21" s="55">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="D21" s="54">
+        <v>0</v>
       </c>
       <c r="E21">
-        <f>B21+C21+D21</f>
-        <v>53</v>
+        <f>D21+C21+B21</f>
+        <v>5</v>
+      </c>
+      <c r="G21" s="53" t="s">
+        <v>61</v>
       </c>
       <c r="H21" s="55">
         <v>0</v>
       </c>
       <c r="I21" s="55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" s="55">
         <v>0</v>
       </c>
       <c r="K21">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>J21+I21+H21</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="53" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="54">
+        <v>64</v>
+      </c>
+      <c r="B22" s="55">
+        <v>1</v>
+      </c>
+      <c r="C22" s="55">
+        <v>2</v>
+      </c>
+      <c r="D22" s="54">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <f>D22+C22+B22</f>
         <v>4</v>
       </c>
-      <c r="C22" s="55">
+      <c r="G22" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="55">
+        <v>0</v>
+      </c>
+      <c r="I22" s="55">
+        <v>0</v>
+      </c>
+      <c r="J22" s="55">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <f>J22+I22+H22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="79">
+        <v>3</v>
+      </c>
+      <c r="C23" s="79">
+        <v>2</v>
+      </c>
+      <c r="D23" s="78">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <f>D23+C23+B23</f>
+        <v>10</v>
+      </c>
+      <c r="G23" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="H23" s="79">
+        <v>0</v>
+      </c>
+      <c r="I23" s="79">
+        <v>0</v>
+      </c>
+      <c r="J23" s="79">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f>J23+I23+H23</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="55">
+        <v>3</v>
+      </c>
+      <c r="C24" s="55">
+        <v>1</v>
+      </c>
+      <c r="D24" s="54">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <f>D24+C24+B24</f>
+        <v>5</v>
+      </c>
+      <c r="G24" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="55">
+        <v>0</v>
+      </c>
+      <c r="I24" s="55">
+        <v>0</v>
+      </c>
+      <c r="J24" s="55">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <f>J24+I24+H24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="55">
         <v>4</v>
       </c>
-      <c r="D22" s="55">
+      <c r="C25" s="55">
+        <v>1</v>
+      </c>
+      <c r="D25" s="54">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <f>D25+C25+B25</f>
+        <v>7</v>
+      </c>
+      <c r="G25" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="55">
+        <v>0</v>
+      </c>
+      <c r="I25" s="55">
+        <v>0</v>
+      </c>
+      <c r="J25" s="55">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <f>J25+I25+H25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="77">
+        <v>5</v>
+      </c>
+      <c r="C26" s="77">
+        <v>5</v>
+      </c>
+      <c r="D26" s="77">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <f>D26+C26+B26</f>
+        <v>15</v>
+      </c>
+      <c r="G26" s="56" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="77">
+        <v>0</v>
+      </c>
+      <c r="I26" s="77">
+        <v>0</v>
+      </c>
+      <c r="J26" s="77">
+        <v>3</v>
+      </c>
+      <c r="K26">
+        <f>J26+I26+H26</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="77">
+        <v>2</v>
+      </c>
+      <c r="C27" s="77">
+        <v>0</v>
+      </c>
+      <c r="D27" s="77">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <f>D27+C27+B27</f>
         <v>4</v>
       </c>
-      <c r="E22">
-        <f>B22+C22+D22</f>
-        <v>12</v>
-      </c>
-      <c r="H22" s="55">
-        <v>0</v>
-      </c>
-      <c r="I22" s="55">
-        <v>0</v>
-      </c>
-      <c r="J22" s="55">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" s="54">
+      <c r="G27" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="77">
+        <v>0</v>
+      </c>
+      <c r="I27" s="77">
+        <v>0</v>
+      </c>
+      <c r="J27" s="77">
         <v>2</v>
       </c>
-      <c r="C23" s="55">
-        <v>1</v>
-      </c>
-      <c r="D23" s="55">
-        <v>4</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="H23" s="55">
-        <v>0</v>
-      </c>
-      <c r="I23" s="55">
-        <v>0</v>
-      </c>
-      <c r="J23" s="55">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" s="57">
-        <v>3</v>
-      </c>
-      <c r="C24" s="58">
-        <v>8</v>
-      </c>
-      <c r="D24" s="58">
+      <c r="K27">
+        <f>J27+I27+H27</f>
         <v>2</v>
       </c>
-      <c r="E24">
-        <f>B24+C24+D24</f>
-        <v>13</v>
-      </c>
-      <c r="H24" s="58">
-        <v>0</v>
-      </c>
-      <c r="I24" s="58">
-        <v>0</v>
-      </c>
-      <c r="J24" s="58">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:A3"/>
+    <mergeCell ref="G1:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6473,8 +6663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC1E50C3-E510-44DF-9648-92EC3D48E3D3}">
   <dimension ref="A2:BM61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F30"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10878,8 +11068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A07BDC3-86C1-49BC-A7E6-7DF335B10BC5}">
   <dimension ref="B2:BB54"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C30"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13611,13 +13801,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="BA6:BB6"/>
+    <mergeCell ref="C5:C6"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="AO6:AP6"/>
-    <mergeCell ref="BA6:BB6"/>
-    <mergeCell ref="C5:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13627,8 +13817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF750BB8-12B1-4DDA-A3C7-AD936B93E529}">
   <dimension ref="A3:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Penyempurnaan KTI Part I
</commit_message>
<xml_diff>
--- a/Perhitungan K-Means K_3.xlsx
+++ b/Perhitungan K-Means K_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CADANGAN SKRIPSI GIT HUB\DATA SKRIPSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E536D8-FD03-4137-BD36-23C4E8E141CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6EBC9E9-47FD-47BB-96FB-42667914C92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{204938CF-0984-440D-97FB-7D0080130912}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="3" xr2:uid="{204938CF-0984-440D-97FB-7D0080130912}"/>
   </bookViews>
   <sheets>
     <sheet name="Normalisasi" sheetId="1" r:id="rId1"/>
@@ -657,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -834,6 +834,9 @@
     <xf numFmtId="2" fontId="8" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -854,15 +857,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1197,53 +1191,53 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C2" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
+      <c r="C2" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J3" s="71" t="s">
+      <c r="J3" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="70">
+      <c r="C5" s="71">
         <v>2021</v>
       </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70">
+      <c r="D5" s="71"/>
+      <c r="E5" s="71">
         <v>2022</v>
       </c>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70" t="s">
+      <c r="F5" s="71"/>
+      <c r="G5" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="70" t="s">
+      <c r="J5" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="70">
+      <c r="K5" s="71">
         <v>2021</v>
       </c>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70">
+      <c r="L5" s="71"/>
+      <c r="M5" s="71">
         <v>2022</v>
       </c>
-      <c r="N5" s="70"/>
+      <c r="N5" s="71"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="70"/>
+      <c r="B6" s="71"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1256,8 +1250,8 @@
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="J6" s="70"/>
+      <c r="G6" s="71"/>
+      <c r="J6" s="71"/>
       <c r="K6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2287,23 +2281,23 @@
       <c r="B32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="70">
+      <c r="C32" s="71">
         <f>C31+D31</f>
         <v>219</v>
       </c>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70">
+      <c r="D32" s="71"/>
+      <c r="E32" s="71">
         <f>E31+F31</f>
         <v>178</v>
       </c>
-      <c r="F32" s="70"/>
+      <c r="F32" s="71"/>
       <c r="J32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K32" s="70"/>
-      <c r="L32" s="70"/>
-      <c r="M32" s="70"/>
-      <c r="N32" s="70"/>
+      <c r="K32" s="71"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="71"/>
+      <c r="N32" s="71"/>
     </row>
     <row r="33" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
@@ -2405,19 +2399,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="C2" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
+      <c r="C2" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
     </row>
     <row r="3" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="H3" s="71" t="s">
+      <c r="H3" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
       <c r="L3" t="s">
         <v>31</v>
       </c>
@@ -2426,12 +2420,12 @@
       </c>
     </row>
     <row r="4" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="L4" s="71" t="s">
+      <c r="L4" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="71"/>
-      <c r="N4" s="71"/>
-      <c r="O4" s="71"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
       <c r="R4" s="27" t="s">
         <v>46</v>
       </c>
@@ -2475,14 +2469,14 @@
       <c r="BG4" s="27"/>
     </row>
     <row r="5" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="70">
+      <c r="C5" s="71">
         <v>2024</v>
       </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70" t="s">
+      <c r="D5" s="71"/>
+      <c r="E5" s="71" t="s">
         <v>28</v>
       </c>
       <c r="H5" s="4"/>
@@ -2565,14 +2559,14 @@
       <c r="BG5" s="27"/>
     </row>
     <row r="6" spans="2:59" x14ac:dyDescent="0.25">
-      <c r="B6" s="70"/>
+      <c r="B6" s="71"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="70"/>
+      <c r="E6" s="71"/>
       <c r="H6" s="4" t="s">
         <v>1</v>
       </c>
@@ -2609,10 +2603,10 @@
       <c r="U6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="V6" s="72" t="s">
+      <c r="V6" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="W6" s="72"/>
+      <c r="W6" s="73"/>
       <c r="Y6" s="2" t="s">
         <v>33</v>
       </c>
@@ -2637,10 +2631,10 @@
       <c r="AG6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="AH6" s="72" t="s">
+      <c r="AH6" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="AI6" s="72"/>
+      <c r="AI6" s="73"/>
       <c r="AK6" s="2" t="s">
         <v>33</v>
       </c>
@@ -2665,10 +2659,10 @@
       <c r="AS6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="AT6" s="72" t="s">
+      <c r="AT6" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="AU6" s="72"/>
+      <c r="AU6" s="73"/>
       <c r="AW6" s="2" t="s">
         <v>33</v>
       </c>
@@ -2686,10 +2680,10 @@
       <c r="BE6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="BF6" s="72" t="s">
+      <c r="BF6" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="BG6" s="72"/>
+      <c r="BG6" s="73"/>
     </row>
     <row r="7" spans="2:59" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -5225,14 +5219,14 @@
       <c r="B32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="70">
+      <c r="C32" s="71">
         <f>C31+D31</f>
         <v>210</v>
       </c>
-      <c r="D32" s="70"/>
+      <c r="D32" s="71"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="70"/>
-      <c r="J32" s="70"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="71"/>
     </row>
     <row r="33" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C33" s="4"/>
@@ -5257,12 +5251,12 @@
     <row r="34" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="H34" s="70"/>
+      <c r="H34" s="71"/>
     </row>
     <row r="35" spans="3:54" x14ac:dyDescent="0.25">
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
-      <c r="H35" s="70"/>
+      <c r="H35" s="71"/>
       <c r="R35" t="s">
         <v>33</v>
       </c>
@@ -5460,12 +5454,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
+      <c r="C1" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H2" t="s">
@@ -5476,22 +5470,22 @@
       </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H3" s="71" t="s">
+      <c r="H3" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="70">
+      <c r="C4" s="71">
         <v>2024</v>
       </c>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70" t="s">
+      <c r="D4" s="71"/>
+      <c r="E4" s="71" t="s">
         <v>28</v>
       </c>
       <c r="H4" t="s">
@@ -5511,14 +5505,14 @@
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="70"/>
+      <c r="B5" s="71"/>
       <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="70"/>
+      <c r="E5" s="71"/>
       <c r="H5" s="2" t="s">
         <v>33</v>
       </c>
@@ -5760,8 +5754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7247C1F-547F-40E3-8593-729479C08754}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5771,7 +5765,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>57</v>
       </c>
       <c r="B1" s="46">
@@ -5783,7 +5777,7 @@
       <c r="D1" s="45">
         <v>2024</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="74" t="s">
         <v>57</v>
       </c>
       <c r="H1" s="47"/>
@@ -5791,7 +5785,7 @@
       <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74"/>
+      <c r="A2" s="75"/>
       <c r="B2" s="49" t="s">
         <v>58</v>
       </c>
@@ -5801,7 +5795,7 @@
       <c r="D2" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="74"/>
+      <c r="G2" s="75"/>
       <c r="H2" s="50" t="s">
         <v>56</v>
       </c>
@@ -5813,7 +5807,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="75"/>
+      <c r="A3" s="76"/>
       <c r="B3" s="52" t="s">
         <v>59</v>
       </c>
@@ -5823,7 +5817,7 @@
       <c r="D3" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="75"/>
+      <c r="G3" s="76"/>
       <c r="H3" s="52" t="s">
         <v>59</v>
       </c>
@@ -5848,8 +5842,11 @@
         <v>5</v>
       </c>
       <c r="E4">
-        <f>D4+C4+B4</f>
+        <f t="shared" ref="E4:E27" si="0">D4+C4+B4</f>
         <v>11</v>
+      </c>
+      <c r="F4" s="70">
+        <v>1</v>
       </c>
       <c r="G4" s="53" t="s">
         <v>62</v>
@@ -5864,7 +5861,7 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <f>J4+I4+H4</f>
+        <f t="shared" ref="K4:K27" si="1">J4+I4+H4</f>
         <v>0</v>
       </c>
     </row>
@@ -5882,8 +5879,11 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <f>D5+C5+B5</f>
+        <f t="shared" si="0"/>
         <v>14</v>
+      </c>
+      <c r="F5" s="70">
+        <v>2</v>
       </c>
       <c r="G5" s="53" t="s">
         <v>67</v>
@@ -5898,7 +5898,7 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <f>J5+I5+H5</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5916,8 +5916,11 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <f>D6+C6+B6</f>
+        <f t="shared" si="0"/>
         <v>21</v>
+      </c>
+      <c r="F6" s="70">
+        <v>3</v>
       </c>
       <c r="G6" s="53" t="s">
         <v>73</v>
@@ -5932,7 +5935,7 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <f>J6+I6+H6</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -5950,8 +5953,11 @@
         <v>22</v>
       </c>
       <c r="E7">
-        <f>D7+C7+B7</f>
+        <f t="shared" si="0"/>
         <v>59</v>
+      </c>
+      <c r="F7" s="70">
+        <v>4</v>
       </c>
       <c r="G7" s="53" t="s">
         <v>68</v>
@@ -5966,7 +5972,7 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <f>J7+I7+H7</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5984,8 +5990,11 @@
         <v>4</v>
       </c>
       <c r="E8">
-        <f>D8+C8+B8</f>
+        <f t="shared" si="0"/>
         <v>8</v>
+      </c>
+      <c r="F8" s="70">
+        <v>5</v>
       </c>
       <c r="G8" s="53" t="s">
         <v>74</v>
@@ -6000,7 +6009,7 @@
         <v>1</v>
       </c>
       <c r="K8">
-        <f>J8+I8+H8</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6018,8 +6027,11 @@
         <v>18</v>
       </c>
       <c r="E9">
-        <f>D9+C9+B9</f>
+        <f t="shared" si="0"/>
         <v>42</v>
+      </c>
+      <c r="F9" s="70">
+        <v>6</v>
       </c>
       <c r="G9" s="53" t="s">
         <v>70</v>
@@ -6034,7 +6046,7 @@
         <v>1</v>
       </c>
       <c r="K9">
-        <f>J9+I9+H9</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6052,8 +6064,11 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <f>D10+C10+B10</f>
+        <f t="shared" si="0"/>
         <v>13</v>
+      </c>
+      <c r="F10" s="70">
+        <v>7</v>
       </c>
       <c r="G10" s="53" t="s">
         <v>76</v>
@@ -6068,7 +6083,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <f>J10+I10+H10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6086,8 +6101,11 @@
         <v>37</v>
       </c>
       <c r="E11">
-        <f>D11+C11+B11</f>
+        <f t="shared" si="0"/>
         <v>188</v>
+      </c>
+      <c r="F11" s="70">
+        <v>8</v>
       </c>
       <c r="G11" s="53" t="s">
         <v>72</v>
@@ -6102,7 +6120,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <f>J11+I11+H11</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6120,8 +6138,11 @@
         <v>9</v>
       </c>
       <c r="E12">
-        <f>D12+C12+B12</f>
+        <f t="shared" si="0"/>
         <v>30</v>
+      </c>
+      <c r="F12" s="70">
+        <v>9</v>
       </c>
       <c r="G12" s="53" t="s">
         <v>75</v>
@@ -6136,7 +6157,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <f>J12+I12+H12</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6154,8 +6175,11 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <f>D13+C13+B13</f>
+        <f t="shared" si="0"/>
         <v>13</v>
+      </c>
+      <c r="F13" s="70">
+        <v>10</v>
       </c>
       <c r="G13" s="56" t="s">
         <v>80</v>
@@ -6170,7 +6194,7 @@
         <v>0</v>
       </c>
       <c r="K13">
-        <f>J13+I13+H13</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6188,8 +6212,11 @@
         <v>2</v>
       </c>
       <c r="E14">
-        <f>D14+C14+B14</f>
+        <f t="shared" si="0"/>
         <v>4</v>
+      </c>
+      <c r="F14" s="70">
+        <v>11</v>
       </c>
       <c r="G14" s="53" t="s">
         <v>63</v>
@@ -6204,7 +6231,7 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <f>J14+I14+H14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6222,8 +6249,11 @@
         <v>13</v>
       </c>
       <c r="E15">
-        <f>D15+C15+B15</f>
-        <v>33</v>
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="F15" s="70">
+        <v>12</v>
       </c>
       <c r="G15" s="53" t="s">
         <v>65</v>
@@ -6238,7 +6268,7 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <f>J15+I15+H15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6256,8 +6286,11 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <f>D16+C16+B16</f>
+        <f t="shared" si="0"/>
         <v>3</v>
+      </c>
+      <c r="F16" s="70">
+        <v>13</v>
       </c>
       <c r="G16" s="53" t="s">
         <v>60</v>
@@ -6272,7 +6305,7 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <f>J16+I16+H16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6290,8 +6323,11 @@
         <v>21</v>
       </c>
       <c r="E17">
-        <f>D17+C17+B17</f>
+        <f t="shared" si="0"/>
         <v>48</v>
+      </c>
+      <c r="F17" s="70">
+        <v>14</v>
       </c>
       <c r="G17" s="53" t="s">
         <v>69</v>
@@ -6306,7 +6342,7 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <f>J17+I17+H17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6324,8 +6360,11 @@
         <v>14</v>
       </c>
       <c r="E18">
-        <f>D18+C18+B18</f>
+        <f t="shared" si="0"/>
         <v>53</v>
+      </c>
+      <c r="F18" s="70">
+        <v>15</v>
       </c>
       <c r="G18" s="53" t="s">
         <v>77</v>
@@ -6340,7 +6379,7 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <f>J18+I18+H18</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6358,8 +6397,11 @@
         <v>4</v>
       </c>
       <c r="E19">
-        <f>D19+C19+B19</f>
+        <f t="shared" si="0"/>
         <v>12</v>
+      </c>
+      <c r="F19" s="70">
+        <v>16</v>
       </c>
       <c r="G19" s="53" t="s">
         <v>78</v>
@@ -6374,7 +6416,7 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <f>J19+I19+H19</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6392,8 +6434,11 @@
         <v>10</v>
       </c>
       <c r="E20">
-        <f>D20+C20+B20</f>
+        <f t="shared" si="0"/>
         <v>30</v>
+      </c>
+      <c r="F20" s="70">
+        <v>17</v>
       </c>
       <c r="G20" s="53" t="s">
         <v>71</v>
@@ -6408,7 +6453,7 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <f>J20+I20+H20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6426,8 +6471,11 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <f>D21+C21+B21</f>
+        <f t="shared" si="0"/>
         <v>5</v>
+      </c>
+      <c r="F21" s="70">
+        <v>18</v>
       </c>
       <c r="G21" s="53" t="s">
         <v>61</v>
@@ -6442,7 +6490,7 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <f>J21+I21+H21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6460,8 +6508,11 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <f>D22+C22+B22</f>
+        <f t="shared" si="0"/>
         <v>4</v>
+      </c>
+      <c r="F22" s="70">
+        <v>19</v>
       </c>
       <c r="G22" s="53" t="s">
         <v>64</v>
@@ -6476,7 +6527,7 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <f>J22+I22+H22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6484,33 +6535,36 @@
       <c r="A23" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="B23" s="79">
+      <c r="B23" s="58">
         <v>3</v>
       </c>
-      <c r="C23" s="79">
+      <c r="C23" s="58">
         <v>2</v>
       </c>
-      <c r="D23" s="78">
+      <c r="D23" s="57">
         <v>5</v>
       </c>
       <c r="E23">
-        <f>D23+C23+B23</f>
+        <f t="shared" si="0"/>
         <v>10</v>
+      </c>
+      <c r="F23" s="70">
+        <v>20</v>
       </c>
       <c r="G23" s="56" t="s">
         <v>86</v>
       </c>
-      <c r="H23" s="79">
-        <v>0</v>
-      </c>
-      <c r="I23" s="79">
-        <v>0</v>
-      </c>
-      <c r="J23" s="79">
+      <c r="H23" s="58">
+        <v>0</v>
+      </c>
+      <c r="I23" s="58">
+        <v>0</v>
+      </c>
+      <c r="J23" s="58">
         <v>1</v>
       </c>
       <c r="K23">
-        <f>J23+I23+H23</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -6528,8 +6582,11 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <f>D24+C24+B24</f>
+        <f t="shared" si="0"/>
         <v>5</v>
+      </c>
+      <c r="F24" s="70">
+        <v>21</v>
       </c>
       <c r="G24" s="53" t="s">
         <v>66</v>
@@ -6544,7 +6601,7 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <f>J24+I24+H24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6562,8 +6619,11 @@
         <v>2</v>
       </c>
       <c r="E25">
-        <f>D25+C25+B25</f>
+        <f t="shared" si="0"/>
         <v>7</v>
+      </c>
+      <c r="F25" s="70">
+        <v>22</v>
       </c>
       <c r="G25" s="53" t="s">
         <v>79</v>
@@ -6578,7 +6638,7 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <f>J25+I25+H25</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -6586,33 +6646,36 @@
       <c r="A26" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="77">
+      <c r="B26" s="70">
         <v>5</v>
       </c>
-      <c r="C26" s="77">
+      <c r="C26" s="70">
         <v>5</v>
       </c>
-      <c r="D26" s="77">
+      <c r="D26" s="70">
         <v>5</v>
       </c>
       <c r="E26">
-        <f>D26+C26+B26</f>
+        <f t="shared" si="0"/>
         <v>15</v>
+      </c>
+      <c r="F26" s="70">
+        <v>23</v>
       </c>
       <c r="G26" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="H26" s="77">
-        <v>0</v>
-      </c>
-      <c r="I26" s="77">
-        <v>0</v>
-      </c>
-      <c r="J26" s="77">
+      <c r="H26" s="70">
+        <v>0</v>
+      </c>
+      <c r="I26" s="70">
+        <v>0</v>
+      </c>
+      <c r="J26" s="70">
         <v>3</v>
       </c>
       <c r="K26">
-        <f>J26+I26+H26</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -6620,33 +6683,36 @@
       <c r="A27" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="77">
+      <c r="B27" s="70">
         <v>2</v>
       </c>
-      <c r="C27" s="77">
-        <v>0</v>
-      </c>
-      <c r="D27" s="77">
+      <c r="C27" s="70">
+        <v>0</v>
+      </c>
+      <c r="D27" s="70">
         <v>2</v>
       </c>
       <c r="E27">
-        <f>D27+C27+B27</f>
+        <f t="shared" si="0"/>
         <v>4</v>
+      </c>
+      <c r="F27" s="70">
+        <v>24</v>
       </c>
       <c r="G27" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="H27" s="77">
-        <v>0</v>
-      </c>
-      <c r="I27" s="77">
-        <v>0</v>
-      </c>
-      <c r="J27" s="77">
+      <c r="H27" s="70">
+        <v>0</v>
+      </c>
+      <c r="I27" s="70">
+        <v>0</v>
+      </c>
+      <c r="J27" s="70">
         <v>2</v>
       </c>
       <c r="K27">
-        <f>J27+I27+H27</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -6679,9 +6745,9 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
       <c r="K2" s="38"/>
       <c r="W2" s="38"/>
       <c r="AQ2" s="38"/>
@@ -6742,12 +6808,12 @@
       <c r="BM3" s="38"/>
     </row>
     <row r="4" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="G4" s="71" t="s">
+      <c r="G4" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
       <c r="K4" s="38"/>
       <c r="M4" s="27" t="s">
         <v>46</v>
@@ -6805,13 +6871,13 @@
       <c r="BM4" s="38"/>
     </row>
     <row r="5" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="71" t="s">
         <v>81</v>
       </c>
       <c r="E5" t="s">
@@ -6896,9 +6962,9 @@
       <c r="BM5" s="38"/>
     </row>
     <row r="6" spans="2:65" x14ac:dyDescent="0.25">
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
       <c r="G6" s="2" t="s">
         <v>33</v>
       </c>
@@ -6987,8 +7053,8 @@
       <c r="AX6" s="35"/>
       <c r="AY6" s="35"/>
       <c r="AZ6" s="36"/>
-      <c r="BA6" s="76"/>
-      <c r="BB6" s="76"/>
+      <c r="BA6" s="77"/>
+      <c r="BB6" s="77"/>
       <c r="BC6" s="38"/>
       <c r="BD6" s="38"/>
       <c r="BE6" s="38"/>
@@ -11083,11 +11149,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="C2" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
+      <c r="C2" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
     </row>
     <row r="3" spans="2:54" x14ac:dyDescent="0.25">
       <c r="G3" t="s">
@@ -11113,12 +11179,12 @@
       <c r="AV3" s="38"/>
     </row>
     <row r="4" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="G4" s="71" t="s">
+      <c r="G4" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
       <c r="M4" s="27" t="s">
         <v>46</v>
       </c>
@@ -11162,13 +11228,13 @@
       <c r="BB4" s="27"/>
     </row>
     <row r="5" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="70" t="s">
+      <c r="C5" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="71" t="s">
         <v>81</v>
       </c>
       <c r="E5" t="s">
@@ -11234,9 +11300,9 @@
       <c r="BB5" s="27"/>
     </row>
     <row r="6" spans="2:54" x14ac:dyDescent="0.25">
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
       <c r="G6" s="2" t="s">
         <v>33</v>
       </c>
@@ -11295,8 +11361,8 @@
       <c r="AL6" s="35"/>
       <c r="AM6" s="35"/>
       <c r="AN6" s="36"/>
-      <c r="AO6" s="76"/>
-      <c r="AP6" s="76"/>
+      <c r="AO6" s="77"/>
+      <c r="AP6" s="77"/>
       <c r="AQ6" s="38"/>
       <c r="AR6" s="32"/>
       <c r="AS6" s="38"/>
@@ -11307,8 +11373,8 @@
       <c r="AX6" s="29"/>
       <c r="AY6" s="29"/>
       <c r="AZ6" s="30"/>
-      <c r="BA6" s="72"/>
-      <c r="BB6" s="72"/>
+      <c r="BA6" s="73"/>
+      <c r="BB6" s="73"/>
     </row>
     <row r="7" spans="2:54" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">

</xml_diff>